<commit_message>
Abänderungen und Zusätze zur Rückschau
</commit_message>
<xml_diff>
--- a/TestprotokolleAlle.xlsx
+++ b/TestprotokolleAlle.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
   <si>
     <t>Testprotokoll</t>
   </si>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -823,7 +823,7 @@
         <v>43258</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -834,7 +834,9 @@
       <c r="B9" s="12">
         <v>43259</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -845,7 +847,7 @@
         <v>43259</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D10" s="5"/>
     </row>
@@ -857,7 +859,7 @@
         <v>43259</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -869,7 +871,7 @@
         <v>43260</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -881,7 +883,7 @@
         <v>43260</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -893,7 +895,7 @@
         <v>43260</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D14" s="5"/>
     </row>
@@ -905,7 +907,7 @@
         <v>43260</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -917,7 +919,7 @@
         <v>43260</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>23</v>
@@ -934,7 +936,7 @@
         <v>43260</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>36</v>
@@ -960,7 +962,7 @@
         <v>43260</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>36</v>
@@ -986,7 +988,7 @@
         <v>43261</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>36</v>
@@ -1239,7 +1241,7 @@
       <c r="B29" s="12">
         <v>43263</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D29" s="5" t="s">

</xml_diff>

<commit_message>
Zusammenfassen aller Test- Protokolle
</commit_message>
<xml_diff>
--- a/TestprotokolleAlle.xlsx
+++ b/TestprotokolleAlle.xlsx
@@ -29,10 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="75">
-  <si>
-    <t>Testprotokoll</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
   <si>
     <t>Welches Ergebnis erwarte ich</t>
   </si>
@@ -56,12 +53,6 @@
 [offen, in Arbeit, erledigt, fehlerhaft]</t>
   </si>
   <si>
-    <t>auf Basis einer fachlichen Analyse</t>
-  </si>
-  <si>
-    <t>und einer Grenzwertanalyse</t>
-  </si>
-  <si>
     <t>Testen ob alle 32 Karten Grafiken angezeigt werden.</t>
   </si>
   <si>
@@ -69,9 +60,6 @@
   </si>
   <si>
     <t>Schiggy fehlte, die Datei war fehlerhaft.</t>
-  </si>
-  <si>
-    <t>erledigt</t>
   </si>
   <si>
     <t>Auch Schiggy wird nun angezeigt.</t>
@@ -91,9 +79,6 @@
     <t>Tim Braumann</t>
   </si>
   <si>
-    <t>Andre Kramp &amp; Tim Braumann</t>
-  </si>
-  <si>
     <t>Smoketest - Darstellung</t>
   </si>
   <si>
@@ -258,6 +243,45 @@
   </si>
   <si>
     <t>Andre Kamp</t>
+  </si>
+  <si>
+    <t>Testen der Logik zum Mischen der Karten</t>
+  </si>
+  <si>
+    <t>Karten sind in zufälliger Reihenfolge in den Decks</t>
+  </si>
+  <si>
+    <t>Testen der json Anbindung</t>
+  </si>
+  <si>
+    <t>Classe Cards erhalt die Korrekte Anzahl und Werte = der Json Quelle</t>
+  </si>
+  <si>
+    <t>Test ob Fehler bei der CompareDiscipline() Logik behoben wurde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test derCompareDiscipline() Logik </t>
+  </si>
+  <si>
+    <t>Korrekte Übergabewerte an RoundDecided()</t>
+  </si>
+  <si>
+    <t>Fehler in der Übergabeparameta syntax</t>
+  </si>
+  <si>
+    <t>Anzeige von gameOverDialog.cs Fenster</t>
+  </si>
+  <si>
+    <t>erledigt &amp; leider noch nicht behoben</t>
+  </si>
+  <si>
+    <t>Testprotokoll der PokeQuet Entwicklung</t>
+  </si>
+  <si>
+    <t>Entwickler:</t>
+  </si>
+  <si>
+    <t>Andre Kramp &amp; Tim Braumann &amp; Benutzergruppen</t>
   </si>
 </sst>
 </file>
@@ -372,7 +396,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -386,8 +410,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -400,6 +428,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -416,19 +447,23 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -730,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,47 +775,52 @@
     <col min="2" max="2" width="24.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2" s="3"/>
       <c r="C2" s="5"/>
-      <c r="E2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>17</v>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>81</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="E3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>19</v>
+      <c r="E3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="5"/>
-      <c r="E4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>65</v>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -789,664 +829,671 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>1</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="13">
         <v>43258</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>2</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="13">
         <v>43259</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="13">
         <v>43259</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>4</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="13">
         <v>43259</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="F11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>5</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="13">
         <v>43260</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>6</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="13">
         <v>43260</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>7</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="13">
         <v>43260</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>8</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="13">
         <v>43260</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>9</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="13">
         <v>43260</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>10</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="13">
         <v>43260</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>11</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="13">
         <v>43260</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>12</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="13">
         <v>43261</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H19" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>13</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="13">
         <v>43261</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" t="s">
         <v>20</v>
-      </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>14</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="13">
         <v>43261</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>15</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="13">
         <v>43261</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" t="s">
         <v>23</v>
       </c>
-      <c r="E22" t="s">
-        <v>21</v>
-      </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>16</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23" s="13">
         <v>43261</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>18</v>
+      <c r="C23" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H23" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>17</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="13">
         <v>43261</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>18</v>
+      <c r="C24" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>18</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="13">
         <v>43261</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="E25" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>19</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26" s="13">
         <v>43263</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G26" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="H26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>20</v>
       </c>
-      <c r="B27" s="12">
+      <c r="B27" s="13">
         <v>43263</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>18</v>
+      <c r="C27" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="F27" t="s">
+        <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="H27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>21</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="13">
         <v>43263</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>18</v>
+      <c r="C28" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="H28" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>22</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="13">
         <v>43263</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>18</v>
+      <c r="C29" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="F29" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="G29" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H29" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>23</v>
       </c>
-      <c r="B30" s="12">
-        <v>43263</v>
+      <c r="B30" s="13">
+        <v>43264</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>18</v>
+        <v>63</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
-        <v>24</v>
-      </c>
-      <c r="B31" s="12">
-        <v>43263</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="5"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
-        <v>25</v>
-      </c>
-      <c r="B32" s="12">
-        <v>43263</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
-        <v>26</v>
-      </c>
-      <c r="B33" s="12">
-        <v>43264</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" t="s">
-        <v>50</v>
-      </c>
-      <c r="F33" t="s">
-        <v>51</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
-        <v>27</v>
-      </c>
-      <c r="B34" s="12">
-        <v>43264</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" t="s">
-        <v>46</v>
-      </c>
-      <c r="H34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
-        <v>28</v>
-      </c>
-      <c r="B35" s="12">
-        <v>43264</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G35" t="s">
-        <v>46</v>
-      </c>
-      <c r="H35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
-        <v>29</v>
-      </c>
-      <c r="B36" s="12">
-        <v>43264</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" t="s">
-        <v>69</v>
-      </c>
-      <c r="F36" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36" t="s">
-        <v>55</v>
-      </c>
-      <c r="H36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
-        <v>30</v>
-      </c>
-      <c r="B37" s="12">
-        <v>43265</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" t="s">
-        <v>63</v>
-      </c>
-      <c r="G37" t="s">
-        <v>64</v>
-      </c>
-      <c r="H37" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="13"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="5"/>
+      <c r="B33" s="13"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="13"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
     </row>
   </sheetData>

</xml_diff>